<commit_message>
read evidences then create
</commit_message>
<xml_diff>
--- a/mapping.xlsx
+++ b/mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mace/Documents/scripts/migrate-tcl-evidences/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D0F9515F-968D-0D42-A986-63EA7F75A863}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0BA6F2A-43A6-F640-9315-4C4531E04F49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3660" yWindow="2660" windowWidth="27640" windowHeight="16940" xr2:uid="{BDF3027E-B7E6-0C40-A7C0-A6B5D900D3B3}"/>
   </bookViews>
@@ -698,7 +698,7 @@
   <dimension ref="A2:D113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>